<commit_message>
Shorten power plant lifetime to allow economic retirements pre-2030
</commit_message>
<xml_diff>
--- a/InputData/elec/MLfPPR/Min Life for Pwr Plnt Rtmnts.xlsx
+++ b/InputData/elec/MLfPPR/Min Life for Pwr Plnt Rtmnts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\MLfPPR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\MLfPPR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA7C5469-9B83-49E8-84E0-DAD6D1CD82B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2629972-E676-42F3-A982-E3273DF7A001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27720" yWindow="3885" windowWidth="28770" windowHeight="17370" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
+    <workbookView xWindow="29880" yWindow="1080" windowWidth="21600" windowHeight="12525" activeTab="1" xr2:uid="{67B50A2A-83E2-40E1-A966-DC033ADD8EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -159,7 +159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -265,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -407,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -417,16 +417,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7A547-DAFD-4CBC-90C6-A86A1413C282}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -434,7 +434,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -451,13 +451,13 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -465,12 +465,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>